<commit_message>
avances en el punto 8
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="01-Tipo Ingreso" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Mes</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>IMP GANANCIAS</t>
+  </si>
+  <si>
+    <t>por mes</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -538,11 +541,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -578,26 +590,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -619,6 +613,27 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,27 +685,29 @@
     <sheetNames>
       <sheetName val="Costos Fijos"/>
       <sheetName val="Costos Variables"/>
+      <sheetName val="Costos legales"/>
+      <sheetName val="Estimacion de pedidos"/>
       <sheetName val="Remuneraciones"/>
       <sheetName val="Amortizaciones "/>
-      <sheetName val="Depreciaciones"/>
       <sheetName val="Impuestos"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="26">
-          <cell r="B26">
-            <v>3175965.1799999997</v>
+        <row r="27">
+          <cell r="B27">
+            <v>3562146.4370000004</v>
           </cell>
-          <cell r="D26">
-            <v>5202054.5880000005</v>
+          <cell r="D27">
+            <v>6014214.9365999997</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -962,7 +979,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,12 +991,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -1000,18 +1017,18 @@
       <c r="G2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="28">
         <v>0.22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="29">
         <v>10500</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="29">
         <f>B3+$B$3*$H$2</f>
         <v>12810</v>
       </c>
@@ -1020,7 +1037,7 @@
         <v>15120</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="D3:E3" si="0">D3+$B$3*$H$2</f>
+        <f t="shared" ref="E3" si="0">D3+$B$3*$H$2</f>
         <v>17430</v>
       </c>
       <c r="I3" s="14"/>
@@ -1029,10 +1046,10 @@
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="29">
         <v>15000</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="29">
         <f>B4+$B$4*$H$2</f>
         <v>18300</v>
       </c>
@@ -1050,10 +1067,10 @@
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="29">
         <v>10</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="29">
         <f>B5+$B$5*$H$2</f>
         <v>12.2</v>
       </c>
@@ -1071,10 +1088,10 @@
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="29">
         <v>1700</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="29">
         <f>B6+$B$6*$H$2</f>
         <v>2074</v>
       </c>
@@ -1092,10 +1109,10 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="29">
         <v>6500</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="29">
         <f>B7+$B$7*$H$2</f>
         <v>7930</v>
       </c>
@@ -1112,10 +1129,10 @@
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="29">
         <v>500</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="29">
         <f>B8+$B$8*$H$2</f>
         <v>610</v>
       </c>
@@ -1132,10 +1149,10 @@
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="29">
         <v>1400</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="29">
         <f>B9+$B$9*$H$2</f>
         <v>1708</v>
       </c>
@@ -1149,14 +1166,14 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="33"/>
+      <c r="D13" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1172,7 +1189,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,31 +1202,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1354,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,16 +1387,16 @@
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+    </row>
+    <row r="2" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1398,8 +1415,11 @@
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
@@ -1419,12 +1439,16 @@
         <f>(('01-Tipo Ingreso'!B6*'02-Volumenes Ingresos'!E4)+('01-Tipo Ingreso'!B7*'02-Volumenes Ingresos'!F4)+('01-Tipo Ingreso'!B8*'02-Volumenes Ingresos'!G4)+('01-Tipo Ingreso'!B9*'02-Volumenes Ingresos'!H4))*6</f>
         <v>253800</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="31">
         <f>SUM(B3:E3)</f>
         <v>1262800</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="27">
+        <f>F3/6</f>
+        <v>210466.66666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>26</v>
       </c>
@@ -1444,12 +1468,16 @@
         <f>(('01-Tipo Ingreso'!C6*'02-Volumenes Ingresos'!E5)+('01-Tipo Ingreso'!C7*'02-Volumenes Ingresos'!F5)+('01-Tipo Ingreso'!C8*'02-Volumenes Ingresos'!G5)+('01-Tipo Ingreso'!C9*'02-Volumenes Ingresos'!H5))*6</f>
         <v>485316</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="31">
         <f>SUM(B4:E4)</f>
         <v>2022516</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="27">
+        <f t="shared" ref="H4:H6" si="0">F4/6</f>
+        <v>337086</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1469,12 +1497,16 @@
         <f>(('01-Tipo Ingreso'!D6*'02-Volumenes Ingresos'!E6)+('01-Tipo Ingreso'!D7*'02-Volumenes Ingresos'!F6)+('01-Tipo Ingreso'!D8*'02-Volumenes Ingresos'!G6)+('01-Tipo Ingreso'!D9*'02-Volumenes Ingresos'!H6))*6</f>
         <v>487296</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="31">
         <f>SUM(B5:E5)</f>
         <v>2919456</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="27">
+        <f t="shared" si="0"/>
+        <v>486576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1494,12 +1526,16 @@
         <f>(('01-Tipo Ingreso'!E6*'02-Volumenes Ingresos'!E7)+('01-Tipo Ingreso'!E7*'02-Volumenes Ingresos'!F7)+('01-Tipo Ingreso'!E8*'02-Volumenes Ingresos'!G7)+('01-Tipo Ingreso'!E9*'02-Volumenes Ingresos'!H7))*6</f>
         <v>434256</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="31">
         <f>SUM(B6:E6)</f>
         <v>4174236</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="27">
+        <f t="shared" si="0"/>
+        <v>695706</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
         <v>22</v>
       </c>
@@ -1510,20 +1546,20 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="32">
         <f>SUM(F3:F4)</f>
         <v>3285316</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="33">
         <f>SUM(F5:F6)</f>
         <v>7093692</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
@@ -1611,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,15 +1661,15 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="39" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="34" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="8">
@@ -1646,16 +1682,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="36">
-        <f>'[1]Costos Fijos'!$B$26</f>
-        <v>3175965.1799999997</v>
-      </c>
-      <c r="C3" s="36">
-        <f>'[1]Costos Fijos'!$D$26</f>
-        <v>5202054.5880000005</v>
+      <c r="B3" s="30">
+        <f>'[1]Costos Fijos'!$B$27</f>
+        <v>3562146.4370000004</v>
+      </c>
+      <c r="C3" s="30">
+        <f>'[1]Costos Fijos'!$D$27</f>
+        <v>6014214.9365999997</v>
       </c>
       <c r="G3" t="s">
         <v>53</v>
@@ -1665,42 +1701,42 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="37">
         <f>B2-B3</f>
-        <v>109350.8200000003</v>
-      </c>
-      <c r="C4" s="43">
+        <v>-276830.43700000038</v>
+      </c>
+      <c r="C4" s="37">
         <f>C2-C3</f>
-        <v>1891637.4119999995</v>
+        <v>1079477.0634000003</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="41">
         <f>-(B4*H3)</f>
-        <v>-38272.787000000098</v>
-      </c>
-      <c r="C5" s="47">
+        <v>96890.652950000134</v>
+      </c>
+      <c r="C5" s="41">
         <f>-(C4*H3)</f>
-        <v>-662073.09419999982</v>
+        <v>-377816.97219000012</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="42">
         <f>SUM(B4:B5)</f>
-        <v>71078.0330000002</v>
-      </c>
-      <c r="C6" s="49">
+        <v>-179939.78405000025</v>
+      </c>
+      <c r="C6" s="43">
         <f>SUM(C4:C5)</f>
-        <v>1229564.3177999998</v>
+        <v>701660.09121000022</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1738,16 +1774,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="33">
+      <c r="B3" s="27">
         <v>-342853</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="27">
         <f>Ganancias!B6</f>
-        <v>71078.0330000002</v>
-      </c>
-      <c r="D3" s="33">
+        <v>-179939.78405000025</v>
+      </c>
+      <c r="D3" s="27">
         <f>Ganancias!C6-Ganancias!C6*0.4</f>
-        <v>737738.59067999991</v>
+        <v>420996.05472600012</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -1767,7 +1803,7 @@
       </c>
       <c r="B9" s="19">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>199222.6072555288</v>
+        <v>-212201.49627366447</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1776,7 +1812,7 @@
       </c>
       <c r="B10" s="20">
         <f>IRR(B3:D3)</f>
-        <v>0.57420364674504731</v>
+        <v>-0.12365207235411702</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1803,11 +1839,11 @@
       </c>
       <c r="C14">
         <f>B14+C3</f>
-        <v>-271774.96699999983</v>
+        <v>-522792.78405000025</v>
       </c>
       <c r="D14">
         <f>C14+D3</f>
-        <v>465963.62368000008</v>
+        <v>-101796.72932400013</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1818,7 +1854,7 @@
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>737738.59067999991</v>
+        <v>420996.05472600012</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -1827,11 +1863,11 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
-        <v>271774.96699999983</v>
+        <v>522792.78405000025</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>4.4206710143683035</v>
+        <v>14.901596673353717</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
avances en costos e ingresos, tir copado
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -12,15 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="01-Tipo Ingreso" sheetId="2" r:id="rId1"/>
-    <sheet name="02-Volumenes Ingresos" sheetId="3" r:id="rId2"/>
-    <sheet name="03-Ingresos" sheetId="1" r:id="rId3"/>
-    <sheet name="04-Gastos" sheetId="6" r:id="rId4"/>
-    <sheet name="Ganancias" sheetId="5" r:id="rId5"/>
-    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId6"/>
+    <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
+    <sheet name="Volumenes Ingresos" sheetId="3" r:id="rId2"/>
+    <sheet name="Ingresos" sheetId="1" r:id="rId3"/>
+    <sheet name="Ganancias" sheetId="5" r:id="rId4"/>
+    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Mes</t>
   </si>
@@ -169,15 +168,6 @@
   </si>
   <si>
     <t>Ingreso</t>
-  </si>
-  <si>
-    <t>Gastos Fijos</t>
-  </si>
-  <si>
-    <t>Gastos Variables</t>
-  </si>
-  <si>
-    <t>Aguinaldos</t>
   </si>
   <si>
     <t>Año 1</t>
@@ -383,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -541,20 +531,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -583,7 +564,6 @@
     <xf numFmtId="17" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -630,9 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,6 +662,7 @@
     <sheetNames>
       <sheetName val="Costos Fijos"/>
       <sheetName val="Costos Variables"/>
+      <sheetName val="Gastos Resultado"/>
       <sheetName val="Costos legales"/>
       <sheetName val="Estimacion de pedidos"/>
       <sheetName val="Remuneraciones"/>
@@ -692,22 +670,23 @@
       <sheetName val="Impuestos"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="27">
-          <cell r="B27">
-            <v>3562146.4370000004</v>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="B4">
+            <v>4836306.8100000005</v>
           </cell>
-          <cell r="D27">
-            <v>6014214.9365999997</v>
+          <cell r="C4">
+            <v>8521710.6059200019</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -979,7 +958,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,12 +970,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -1006,39 +985,39 @@
         <v>25</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>0.22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="29">
-        <v>10500</v>
-      </c>
-      <c r="C3" s="29">
+      <c r="B3" s="28">
+        <v>16000</v>
+      </c>
+      <c r="C3" s="28">
         <f>B3+$B$3*$H$2</f>
-        <v>12810</v>
+        <v>19520</v>
       </c>
       <c r="D3" s="8">
         <f>C3+$B$3*$H$2</f>
-        <v>15120</v>
+        <v>23040</v>
       </c>
       <c r="E3" s="8">
         <f t="shared" ref="E3" si="0">D3+$B$3*$H$2</f>
-        <v>17430</v>
+        <v>26560</v>
       </c>
       <c r="I3" s="14"/>
     </row>
@@ -1046,20 +1025,20 @@
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29">
-        <v>15000</v>
-      </c>
-      <c r="C4" s="29">
+      <c r="B4" s="28">
+        <v>19700</v>
+      </c>
+      <c r="C4" s="28">
         <f>B4+$B$4*$H$2</f>
-        <v>18300</v>
+        <v>24034</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" ref="D4:E4" si="1">C4+$B$4*$H$2</f>
-        <v>21600</v>
+        <v>28368</v>
       </c>
       <c r="E4" s="8">
         <f t="shared" si="1"/>
-        <v>24900</v>
+        <v>32702</v>
       </c>
       <c r="I4" s="14"/>
     </row>
@@ -1067,20 +1046,20 @@
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="29">
-        <v>10</v>
-      </c>
-      <c r="C5" s="29">
+      <c r="B5" s="28">
+        <v>16</v>
+      </c>
+      <c r="C5" s="28">
         <f>B5+$B$5*$H$2</f>
-        <v>12.2</v>
+        <v>19.52</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" ref="D5:E5" si="2">C5+$B$5*$H$2</f>
-        <v>14.399999999999999</v>
+        <v>23.04</v>
       </c>
       <c r="E5" s="8">
         <f t="shared" si="2"/>
-        <v>16.599999999999998</v>
+        <v>26.56</v>
       </c>
       <c r="I5" s="14"/>
     </row>
@@ -1088,20 +1067,20 @@
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="29">
-        <v>1700</v>
-      </c>
-      <c r="C6" s="29">
+      <c r="B6" s="28">
+        <v>2000</v>
+      </c>
+      <c r="C6" s="28">
         <f>B6+$B$6*$H$2</f>
-        <v>2074</v>
+        <v>2440</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" ref="D6:E6" si="3">C6+$B$6*$H$2</f>
-        <v>2448</v>
+        <v>2880</v>
       </c>
       <c r="E6" s="8">
         <f t="shared" si="3"/>
-        <v>2822</v>
+        <v>3320</v>
       </c>
       <c r="I6" s="14"/>
     </row>
@@ -1109,71 +1088,71 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="29">
-        <v>6500</v>
-      </c>
-      <c r="C7" s="29">
+      <c r="B7" s="28">
+        <v>7500</v>
+      </c>
+      <c r="C7" s="28">
         <f>B7+$B$7*$H$2</f>
-        <v>7930</v>
+        <v>9150</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" ref="D7:E7" si="4">C7+$B$7*$H$2</f>
-        <v>9360</v>
+        <v>10800</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="4"/>
-        <v>10790</v>
+        <v>12450</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="29">
-        <v>500</v>
-      </c>
-      <c r="C8" s="29">
+      <c r="B8" s="28">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="28">
         <f>B8+$B$8*$H$2</f>
-        <v>610</v>
+        <v>1220</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" ref="D8:E8" si="5">C8+$B$8*$H$2</f>
-        <v>720</v>
+        <v>1440</v>
       </c>
       <c r="E8" s="8">
         <f t="shared" si="5"/>
-        <v>830</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="29">
-        <v>1400</v>
-      </c>
-      <c r="C9" s="29">
+      <c r="B9" s="28">
+        <v>3300</v>
+      </c>
+      <c r="C9" s="28">
         <f>B9+$B$9*$H$2</f>
-        <v>1708</v>
+        <v>4026</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" ref="D9:E9" si="6">C9+$B$9*$H$2</f>
-        <v>2016</v>
+        <v>4752</v>
       </c>
       <c r="E9" s="8">
         <f t="shared" si="6"/>
-        <v>2324</v>
+        <v>5478</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="27"/>
+      <c r="D13" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1189,7 +1168,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,31 +1181,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1259,13 +1238,13 @@
         <v>25</v>
       </c>
       <c r="B4" s="17">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="17">
-        <v>1000</v>
+        <v>1560</v>
       </c>
       <c r="E4" s="17">
         <v>4</v>
@@ -1285,10 +1264,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="17">
         <v>3000</v>
@@ -1311,10 +1290,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="12">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C6" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="6">
         <v>4000</v>
@@ -1337,13 +1316,13 @@
         <v>28</v>
       </c>
       <c r="B7" s="12">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="E7" s="6">
         <v>5</v>
@@ -1374,7 +1353,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,16 +1364,17 @@
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1415,8 +1395,8 @@
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="50" t="s">
-        <v>54</v>
+      <c r="H2" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1424,28 +1404,28 @@
         <v>25</v>
       </c>
       <c r="B3" s="16">
-        <f>('01-Tipo Ingreso'!B3*'02-Volumenes Ingresos'!B4)*6</f>
-        <v>819000</v>
+        <f>('Tipo Ingreso'!B3*'Volumenes Ingresos'!B4)*6</f>
+        <v>1056000</v>
       </c>
       <c r="C3" s="16">
-        <f>('01-Tipo Ingreso'!B4*'02-Volumenes Ingresos'!C4)*6</f>
-        <v>180000</v>
+        <f>('Tipo Ingreso'!B4*'Volumenes Ingresos'!C4)*6</f>
+        <v>472800</v>
       </c>
       <c r="D3" s="16">
-        <f>('01-Tipo Ingreso'!B5*'02-Volumenes Ingresos'!D4)</f>
-        <v>10000</v>
+        <f>('Tipo Ingreso'!B5*'Volumenes Ingresos'!D4)</f>
+        <v>24960</v>
       </c>
       <c r="E3" s="16">
-        <f>(('01-Tipo Ingreso'!B6*'02-Volumenes Ingresos'!E4)+('01-Tipo Ingreso'!B7*'02-Volumenes Ingresos'!F4)+('01-Tipo Ingreso'!B8*'02-Volumenes Ingresos'!G4)+('01-Tipo Ingreso'!B9*'02-Volumenes Ingresos'!H4))*6</f>
-        <v>253800</v>
-      </c>
-      <c r="F3" s="31">
+        <f>(('Tipo Ingreso'!B6*'Volumenes Ingresos'!E4)+('Tipo Ingreso'!B7*'Volumenes Ingresos'!F4)+('Tipo Ingreso'!B8*'Volumenes Ingresos'!G4)+('Tipo Ingreso'!B9*'Volumenes Ingresos'!H4))*6</f>
+        <v>357000</v>
+      </c>
+      <c r="F3" s="30">
         <f>SUM(B3:E3)</f>
-        <v>1262800</v>
-      </c>
-      <c r="H3" s="27">
+        <v>1910760</v>
+      </c>
+      <c r="H3" s="30">
         <f>F3/6</f>
-        <v>210466.66666666666</v>
+        <v>318460</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1453,28 +1433,28 @@
         <v>26</v>
       </c>
       <c r="B4" s="16">
-        <f>('01-Tipo Ingreso'!C3*'02-Volumenes Ingresos'!B5)*6</f>
-        <v>768600</v>
+        <f>('Tipo Ingreso'!C3*'Volumenes Ingresos'!B5)*6</f>
+        <v>1054080</v>
       </c>
       <c r="C4" s="16">
-        <f>6*'01-Tipo Ingreso'!C4*'02-Volumenes Ingresos'!C5</f>
-        <v>549000</v>
+        <f>6*'Tipo Ingreso'!C4*'Volumenes Ingresos'!C5</f>
+        <v>865224</v>
       </c>
       <c r="D4" s="16">
-        <f>('01-Tipo Ingreso'!C5*'02-Volumenes Ingresos'!D5)*6</f>
-        <v>219600</v>
+        <f>('Tipo Ingreso'!C5*'Volumenes Ingresos'!D5)*6</f>
+        <v>351360</v>
       </c>
       <c r="E4" s="16">
-        <f>(('01-Tipo Ingreso'!C6*'02-Volumenes Ingresos'!E5)+('01-Tipo Ingreso'!C7*'02-Volumenes Ingresos'!F5)+('01-Tipo Ingreso'!C8*'02-Volumenes Ingresos'!G5)+('01-Tipo Ingreso'!C9*'02-Volumenes Ingresos'!H5))*6</f>
-        <v>485316</v>
-      </c>
-      <c r="F4" s="31">
+        <f>(('Tipo Ingreso'!C6*'Volumenes Ingresos'!E5)+('Tipo Ingreso'!C7*'Volumenes Ingresos'!F5)+('Tipo Ingreso'!C8*'Volumenes Ingresos'!G5)+('Tipo Ingreso'!C9*'Volumenes Ingresos'!H5))*6</f>
+        <v>663192</v>
+      </c>
+      <c r="F4" s="30">
         <f>SUM(B4:E4)</f>
-        <v>2022516</v>
-      </c>
-      <c r="H4" s="27">
+        <v>2933856</v>
+      </c>
+      <c r="H4" s="30">
         <f t="shared" ref="H4:H6" si="0">F4/6</f>
-        <v>337086</v>
+        <v>488976</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,28 +1462,28 @@
         <v>27</v>
       </c>
       <c r="B5" s="8">
-        <f>('01-Tipo Ingreso'!D3*'02-Volumenes Ingresos'!B6)*6</f>
-        <v>1179360</v>
+        <f>('Tipo Ingreso'!D3*'Volumenes Ingresos'!B6)*6</f>
+        <v>3041280</v>
       </c>
       <c r="C5" s="8">
-        <f>'01-Tipo Ingreso'!D4*'02-Volumenes Ingresos'!C6*6</f>
-        <v>907200</v>
+        <f>'Tipo Ingreso'!D4*'Volumenes Ingresos'!C6*6</f>
+        <v>1361664</v>
       </c>
       <c r="D5" s="8">
-        <f>('01-Tipo Ingreso'!D5*'02-Volumenes Ingresos'!D6)*6</f>
-        <v>345599.99999999994</v>
+        <f>('Tipo Ingreso'!D5*'Volumenes Ingresos'!D6)*6</f>
+        <v>552960</v>
       </c>
       <c r="E5" s="8">
-        <f>(('01-Tipo Ingreso'!D6*'02-Volumenes Ingresos'!E6)+('01-Tipo Ingreso'!D7*'02-Volumenes Ingresos'!F6)+('01-Tipo Ingreso'!D8*'02-Volumenes Ingresos'!G6)+('01-Tipo Ingreso'!D9*'02-Volumenes Ingresos'!H6))*6</f>
-        <v>487296</v>
-      </c>
-      <c r="F5" s="31">
+        <f>(('Tipo Ingreso'!D6*'Volumenes Ingresos'!E6)+('Tipo Ingreso'!D7*'Volumenes Ingresos'!F6)+('Tipo Ingreso'!D8*'Volumenes Ingresos'!G6)+('Tipo Ingreso'!D9*'Volumenes Ingresos'!H6))*6</f>
+        <v>698976</v>
+      </c>
+      <c r="F5" s="30">
         <f>SUM(B5:E5)</f>
-        <v>2919456</v>
-      </c>
-      <c r="H5" s="27">
+        <v>5654880</v>
+      </c>
+      <c r="H5" s="30">
         <f t="shared" si="0"/>
-        <v>486576</v>
+        <v>942480</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1511,52 +1491,52 @@
         <v>28</v>
       </c>
       <c r="B6" s="8">
-        <f>('01-Tipo Ingreso'!E3*'02-Volumenes Ingresos'!B7)*6</f>
-        <v>2196180</v>
+        <f>('Tipo Ingreso'!E3*'Volumenes Ingresos'!B7)*6</f>
+        <v>3187200</v>
       </c>
       <c r="C6" s="8">
-        <f>'01-Tipo Ingreso'!E4*'02-Volumenes Ingresos'!C7*6</f>
-        <v>1344600</v>
+        <f>'Tipo Ingreso'!E4*'Volumenes Ingresos'!C7*6</f>
+        <v>1962120</v>
       </c>
       <c r="D6" s="8">
-        <f>('01-Tipo Ingreso'!E5*'02-Volumenes Ingresos'!D7)*6</f>
-        <v>199199.99999999994</v>
+        <f>('Tipo Ingreso'!E5*'Volumenes Ingresos'!D7)*6</f>
+        <v>334656</v>
       </c>
       <c r="E6" s="8">
-        <f>(('01-Tipo Ingreso'!E6*'02-Volumenes Ingresos'!E7)+('01-Tipo Ingreso'!E7*'02-Volumenes Ingresos'!F7)+('01-Tipo Ingreso'!E8*'02-Volumenes Ingresos'!G7)+('01-Tipo Ingreso'!E9*'02-Volumenes Ingresos'!H7))*6</f>
-        <v>434256</v>
-      </c>
-      <c r="F6" s="31">
+        <f>(('Tipo Ingreso'!E6*'Volumenes Ingresos'!E7)+('Tipo Ingreso'!E7*'Volumenes Ingresos'!F7)+('Tipo Ingreso'!E8*'Volumenes Ingresos'!G7)+('Tipo Ingreso'!E9*'Volumenes Ingresos'!H7))*6</f>
+        <v>679272</v>
+      </c>
+      <c r="F6" s="30">
         <f>SUM(B6:E6)</f>
-        <v>4174236</v>
-      </c>
-      <c r="H6" s="27">
-        <f t="shared" si="0"/>
-        <v>695706</v>
+        <v>6163248</v>
+      </c>
+      <c r="H6" s="30">
+        <f>F6/6</f>
+        <v>1027208</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="21">
         <v>2016</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>2017</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <f>SUM(F3:F4)</f>
-        <v>3285316</v>
-      </c>
-      <c r="D11" s="33">
+        <v>4844616</v>
+      </c>
+      <c r="D11" s="32">
         <f>SUM(F5:F6)</f>
-        <v>7093692</v>
+        <v>11818128</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1571,73 +1551,100 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="8">
+        <f>Ingresos!C11</f>
+        <v>4844616</v>
+      </c>
+      <c r="C2" s="8">
+        <f>Ingresos!D11</f>
+        <v>11818128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2">
-        <v>2086920</v>
-      </c>
-      <c r="C2">
-        <f>B2+(B2*'01-Tipo Ingreso'!I4)+503577</f>
-        <v>2590497</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>420000</v>
-      </c>
-      <c r="C3">
-        <f>B3+(B3*'01-Tipo Ingreso'!I5)+128250</f>
-        <v>548250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="29">
+        <f>'[1]Gastos Resultado'!$B$4</f>
+        <v>4836306.8100000005</v>
+      </c>
+      <c r="C3" s="29">
+        <f>'[1]Gastos Resultado'!$C$4</f>
+        <v>8521710.6059200019</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="36">
+        <f>B2-B3</f>
+        <v>8309.1899999994785</v>
+      </c>
+      <c r="C4" s="36">
+        <f>C2-C3</f>
+        <v>3296417.3940799981</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="40">
+        <f>-(B4*H3)</f>
+        <v>-2908.2164999998172</v>
+      </c>
+      <c r="C5" s="40">
+        <f>-(C4*H3)</f>
+        <v>-1153746.0879279992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B4">
-        <v>122168</v>
-      </c>
-      <c r="C4">
-        <v>171035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="18">
-        <f>SUM(B2:B4)</f>
-        <v>2629088</v>
-      </c>
-      <c r="C5" s="18">
-        <f>SUM(C2:C4)</f>
-        <v>3309782</v>
-      </c>
-    </row>
+      <c r="B6" s="41">
+        <f>SUM(B4:B5)</f>
+        <v>5400.9734999996617</v>
+      </c>
+      <c r="C6" s="42">
+        <f>SUM(C4:C5)</f>
+        <v>2142671.3061519992</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1645,117 +1652,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="8">
-        <f>'03-Ingresos'!C11</f>
-        <v>3285316</v>
-      </c>
-      <c r="C2" s="8">
-        <f>'03-Ingresos'!D11</f>
-        <v>7093692</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="30">
-        <f>'[1]Costos Fijos'!$B$27</f>
-        <v>3562146.4370000004</v>
-      </c>
-      <c r="C3" s="30">
-        <f>'[1]Costos Fijos'!$D$27</f>
-        <v>6014214.9365999997</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="14">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="37">
-        <f>B2-B3</f>
-        <v>-276830.43700000038</v>
-      </c>
-      <c r="C4" s="37">
-        <f>C2-C3</f>
-        <v>1079477.0634000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="41">
-        <f>-(B4*H3)</f>
-        <v>96890.652950000134</v>
-      </c>
-      <c r="C5" s="41">
-        <f>-(C4*H3)</f>
-        <v>-377816.97219000012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="42">
-        <f>SUM(B4:B5)</f>
-        <v>-179939.78405000025</v>
-      </c>
-      <c r="C6" s="43">
-        <f>SUM(C4:C5)</f>
-        <v>701660.09121000022</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1774,45 +1680,45 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="27">
-        <v>-342853</v>
-      </c>
-      <c r="C3" s="27">
+      <c r="B3" s="26">
+        <v>-358000</v>
+      </c>
+      <c r="C3" s="26">
         <f>Ganancias!B6</f>
-        <v>-179939.78405000025</v>
-      </c>
-      <c r="D3" s="27">
-        <f>Ganancias!C6-Ganancias!C6*0.4</f>
-        <v>420996.05472600012</v>
+        <v>5400.9734999996617</v>
+      </c>
+      <c r="D3" s="26">
+        <f>Ganancias!C6-Ganancias!C6*0.6</f>
+        <v>857068.52246079966</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="20">
+        <v>38</v>
+      </c>
+      <c r="I4" s="19">
         <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="19">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>-212201.49627366447</v>
+        <v>209217.15347685327</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="20">
+        <v>40</v>
+      </c>
+      <c r="B10" s="19">
         <f>IRR(B3:D3)</f>
-        <v>-0.12365207235411702</v>
+        <v>0.55483219553534924</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1831,30 +1737,30 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <f>B3</f>
-        <v>-342853</v>
+        <v>-358000</v>
       </c>
       <c r="C14">
         <f>B14+C3</f>
-        <v>-522792.78405000025</v>
+        <v>-352599.02650000033</v>
       </c>
       <c r="D14">
         <f>C14+D3</f>
-        <v>-101796.72932400013</v>
+        <v>504469.49596079934</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>420996.05472600012</v>
+        <v>857068.52246079966</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -1863,19 +1769,19 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
-        <v>522792.78405000025</v>
+        <v>352599.02650000033</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>14.901596673353717</v>
+        <v>4.9368145102931704</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglos en los ingresos y costos
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
@@ -675,10 +675,10 @@
       <sheetData sheetId="2">
         <row r="4">
           <cell r="B4">
-            <v>4836306.8100000005</v>
+            <v>4794714.41</v>
           </cell>
           <cell r="C4">
-            <v>8521710.6059200019</v>
+            <v>8309827.3409200003</v>
           </cell>
         </row>
       </sheetData>
@@ -958,7 +958,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,10 +1290,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6">
         <v>4000</v>
@@ -1316,10 +1316,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="6">
         <v>2100</v>
@@ -1352,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1453,7 @@
         <v>2933856</v>
       </c>
       <c r="H4" s="30">
-        <f t="shared" ref="H4:H6" si="0">F4/6</f>
+        <f t="shared" ref="H4:H5" si="0">F4/6</f>
         <v>488976</v>
       </c>
     </row>
@@ -1463,11 +1463,11 @@
       </c>
       <c r="B5" s="8">
         <f>('Tipo Ingreso'!D3*'Volumenes Ingresos'!B6)*6</f>
-        <v>3041280</v>
+        <v>3179520</v>
       </c>
       <c r="C5" s="8">
         <f>'Tipo Ingreso'!D4*'Volumenes Ingresos'!C6*6</f>
-        <v>1361664</v>
+        <v>1191456</v>
       </c>
       <c r="D5" s="8">
         <f>('Tipo Ingreso'!D5*'Volumenes Ingresos'!D6)*6</f>
@@ -1479,11 +1479,11 @@
       </c>
       <c r="F5" s="30">
         <f>SUM(B5:E5)</f>
-        <v>5654880</v>
+        <v>5622912</v>
       </c>
       <c r="H5" s="30">
         <f t="shared" si="0"/>
-        <v>942480</v>
+        <v>937152</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,11 +1492,11 @@
       </c>
       <c r="B6" s="8">
         <f>('Tipo Ingreso'!E3*'Volumenes Ingresos'!B7)*6</f>
-        <v>3187200</v>
+        <v>3346560</v>
       </c>
       <c r="C6" s="8">
         <f>'Tipo Ingreso'!E4*'Volumenes Ingresos'!C7*6</f>
-        <v>1962120</v>
+        <v>1765908</v>
       </c>
       <c r="D6" s="8">
         <f>('Tipo Ingreso'!E5*'Volumenes Ingresos'!D7)*6</f>
@@ -1508,11 +1508,11 @@
       </c>
       <c r="F6" s="30">
         <f>SUM(B6:E6)</f>
-        <v>6163248</v>
+        <v>6126396</v>
       </c>
       <c r="H6" s="30">
         <f>F6/6</f>
-        <v>1027208</v>
+        <v>1021066</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="D11" s="32">
         <f>SUM(F5:F6)</f>
-        <v>11818128</v>
+        <v>11749308</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="C2" s="8">
         <f>Ingresos!D11</f>
-        <v>11818128</v>
+        <v>11749308</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,11 +1592,11 @@
       </c>
       <c r="B3" s="29">
         <f>'[1]Gastos Resultado'!$B$4</f>
-        <v>4836306.8100000005</v>
+        <v>4794714.41</v>
       </c>
       <c r="C3" s="29">
         <f>'[1]Gastos Resultado'!$C$4</f>
-        <v>8521710.6059200019</v>
+        <v>8309827.3409200003</v>
       </c>
       <c r="G3" t="s">
         <v>50</v>
@@ -1611,11 +1611,11 @@
       </c>
       <c r="B4" s="36">
         <f>B2-B3</f>
-        <v>8309.1899999994785</v>
+        <v>49901.589999999851</v>
       </c>
       <c r="C4" s="36">
         <f>C2-C3</f>
-        <v>3296417.3940799981</v>
+        <v>3439480.6590799997</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1624,11 +1624,11 @@
       </c>
       <c r="B5" s="40">
         <f>-(B4*H3)</f>
-        <v>-2908.2164999998172</v>
+        <v>-17465.556499999948</v>
       </c>
       <c r="C5" s="40">
         <f>-(C4*H3)</f>
-        <v>-1153746.0879279992</v>
+        <v>-1203818.2306779998</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1637,11 +1637,11 @@
       </c>
       <c r="B6" s="41">
         <f>SUM(B4:B5)</f>
-        <v>5400.9734999996617</v>
+        <v>32436.033499999903</v>
       </c>
       <c r="C6" s="42">
         <f>SUM(C4:C5)</f>
-        <v>2142671.3061519992</v>
+        <v>2235662.4284020001</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1654,13 +1654,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1685,11 +1686,11 @@
       </c>
       <c r="C3" s="26">
         <f>Ganancias!B6</f>
-        <v>5400.9734999996617</v>
+        <v>32436.033499999903</v>
       </c>
       <c r="D3" s="26">
         <f>Ganancias!C6-Ganancias!C6*0.6</f>
-        <v>857068.52246079966</v>
+        <v>894264.97136080009</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
@@ -1709,7 +1710,7 @@
       </c>
       <c r="B9" s="18">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>209217.15347685327</v>
+        <v>255552.68782378791</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1718,7 +1719,7 @@
       </c>
       <c r="B10" s="19">
         <f>IRR(B3:D3)</f>
-        <v>0.55483219553534924</v>
+        <v>0.62644026617705229</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1745,11 +1746,11 @@
       </c>
       <c r="C14">
         <f>B14+C3</f>
-        <v>-352599.02650000033</v>
+        <v>-325563.9665000001</v>
       </c>
       <c r="D14">
         <f>C14+D3</f>
-        <v>504469.49596079934</v>
+        <v>568701.00486079999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1760,7 +1761,7 @@
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>857068.52246079966</v>
+        <v>894264.97136080009</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -1769,11 +1770,11 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
-        <v>352599.02650000033</v>
+        <v>325563.9665000001</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>4.9368145102931704</v>
+        <v>4.3686912974519014</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
punto 8 casi finalizado
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>se le restó inflacion</t>
   </si>
   <si>
-    <t>5 meses</t>
-  </si>
-  <si>
     <t>Semestre 2 -2016</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>por mes</t>
+  </si>
+  <si>
+    <t>6 meses</t>
   </si>
 </sst>
 </file>
@@ -675,10 +675,10 @@
       <sheetData sheetId="2">
         <row r="4">
           <cell r="B4">
-            <v>4794714.41</v>
+            <v>4822844.05</v>
           </cell>
           <cell r="C4">
-            <v>8309827.3409200003</v>
+            <v>8767153.8409200013</v>
           </cell>
         </row>
       </sheetData>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +971,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
@@ -985,13 +985,13 @@
         <v>25</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>47</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>23</v>
@@ -1350,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1367,7 @@
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="48" t="s">
         <v>19</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1396,10 +1396,10 @@
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>318460</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>26</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>488976</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1485,8 +1485,9 @@
         <f t="shared" si="0"/>
         <v>937152</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="26"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1515,7 +1516,7 @@
         <v>1021066</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20" t="s">
         <v>22</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>30</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>11749308</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
@@ -1554,7 +1555,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,14 +1593,14 @@
       </c>
       <c r="B3" s="29">
         <f>'[1]Gastos Resultado'!$B$4</f>
-        <v>4794714.41</v>
+        <v>4822844.05</v>
       </c>
       <c r="C3" s="29">
         <f>'[1]Gastos Resultado'!$C$4</f>
-        <v>8309827.3409200003</v>
+        <v>8767153.8409200013</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3" s="14">
         <v>0.35</v>
@@ -1611,11 +1612,11 @@
       </c>
       <c r="B4" s="36">
         <f>B2-B3</f>
-        <v>49901.589999999851</v>
+        <v>21771.950000000186</v>
       </c>
       <c r="C4" s="36">
         <f>C2-C3</f>
-        <v>3439480.6590799997</v>
+        <v>2982154.1590799987</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1624,11 +1625,11 @@
       </c>
       <c r="B5" s="40">
         <f>-(B4*H3)</f>
-        <v>-17465.556499999948</v>
+        <v>-7620.1825000000645</v>
       </c>
       <c r="C5" s="40">
         <f>-(C4*H3)</f>
-        <v>-1203818.2306779998</v>
+        <v>-1043753.9556779995</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1637,11 +1638,11 @@
       </c>
       <c r="B6" s="41">
         <f>SUM(B4:B5)</f>
-        <v>32436.033499999903</v>
+        <v>14151.767500000122</v>
       </c>
       <c r="C6" s="42">
         <f>SUM(C4:C5)</f>
-        <v>2235662.4284020001</v>
+        <v>1938400.2034019991</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1654,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,11 +1687,11 @@
       </c>
       <c r="C3" s="26">
         <f>Ganancias!B6</f>
-        <v>32436.033499999903</v>
+        <v>14151.767500000122</v>
       </c>
       <c r="D3" s="26">
         <f>Ganancias!C6-Ganancias!C6*0.6</f>
-        <v>894264.97136080009</v>
+        <v>775360.08136079973</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
@@ -1710,7 +1711,7 @@
       </c>
       <c r="B9" s="18">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>255552.68782378791</v>
+        <v>162650.296210161</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1719,7 +1720,7 @@
       </c>
       <c r="B10" s="19">
         <f>IRR(B3:D3)</f>
-        <v>0.62644026617705229</v>
+        <v>0.49156697476814148</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,11 +1747,11 @@
       </c>
       <c r="C14">
         <f>B14+C3</f>
-        <v>-325563.9665000001</v>
+        <v>-343848.23249999987</v>
       </c>
       <c r="D14">
         <f>C14+D3</f>
-        <v>568701.00486079999</v>
+        <v>431511.84886079986</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1761,7 +1762,7 @@
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>894264.97136080009</v>
+        <v>775360.08136079973</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -1770,11 +1771,11 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
-        <v>325563.9665000001</v>
+        <v>343848.23249999987</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>4.3686912974519014</v>
+        <v>5.3216291232820847</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1782,7 +1783,7 @@
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avances, casi terminado. arreglado
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
     <sheet name="Volumenes Ingresos" sheetId="3" r:id="rId2"/>
     <sheet name="Ingresos" sheetId="1" r:id="rId3"/>
     <sheet name="Ganancias" sheetId="5" r:id="rId4"/>
-    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId5"/>
+    <sheet name="Modelo Financiero" sheetId="6" r:id="rId5"/>
+    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>Mes</t>
   </si>
@@ -209,9 +211,6 @@
     <t>1 año</t>
   </si>
   <si>
-    <t>se le restó inflacion</t>
-  </si>
-  <si>
     <t>Semestre 2 -2016</t>
   </si>
   <si>
@@ -231,6 +230,45 @@
   </si>
   <si>
     <t>6 meses</t>
+  </si>
+  <si>
+    <t>Fondo Inicial</t>
+  </si>
+  <si>
+    <t>Inversion Inicial</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Impuesto a las ganancias (35%)</t>
+  </si>
+  <si>
+    <t>Año 2016</t>
+  </si>
+  <si>
+    <t>Año 2017</t>
+  </si>
+  <si>
+    <t>Flujo de Fondos</t>
+  </si>
+  <si>
+    <t>Flujo de fondos</t>
+  </si>
+  <si>
+    <t>Resultado Acumulado</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>1 año y 3 meses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ganancias Totales </t>
+  </si>
+  <si>
+    <t>Fondo Final</t>
   </si>
 </sst>
 </file>
@@ -241,7 +279,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]&quot;$&quot;\ \-#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,8 +312,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,8 +438,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -531,11 +621,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -611,6 +721,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,6 +827,39 @@
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Inversión inicial P1"/>
+      <sheetName val="Inversión Inicial PUM"/>
+      <sheetName val="Costos fijos P1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="E3">
+            <v>99500</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="E29">
+            <v>360838</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="E31">
+            <v>500838</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -957,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -971,7 +1144,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
@@ -985,13 +1158,13 @@
         <v>25</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>23</v>
@@ -1396,7 +1569,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1600,7 +1773,7 @@
         <v>8767153.8409200013</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="14">
         <v>0.35</v>
@@ -1653,10 +1826,312 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="57">
+        <f>'[2]Inversión Inicial PUM'!$E$31</f>
+        <v>500838</v>
+      </c>
+      <c r="C2" s="57">
+        <f>B10</f>
+        <v>154151.76750000013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="58">
+        <f>-'[2]Inversión Inicial PUM'!$E$29</f>
+        <v>-360838</v>
+      </c>
+      <c r="C3" s="58">
+        <f>-('[2]Inversión Inicial PUM'!$E$3+'[2]Inversión Inicial PUM'!$E$3*40%)</f>
+        <v>-139300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="59">
+        <f>B2+B3</f>
+        <v>140000</v>
+      </c>
+      <c r="C4" s="59">
+        <f>C2+C3</f>
+        <v>14851.767500000133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="60">
+        <f>Ganancias!B2</f>
+        <v>4844616</v>
+      </c>
+      <c r="C5" s="60">
+        <f>Ganancias!C2</f>
+        <v>11749308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="58">
+        <f>-Ganancias!B3</f>
+        <v>-4822844.05</v>
+      </c>
+      <c r="C6" s="58">
+        <f>-Ganancias!C3</f>
+        <v>-8767153.8409200013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="61">
+        <f>B5+B6</f>
+        <v>21771.950000000186</v>
+      </c>
+      <c r="C7" s="61">
+        <f>C5+C6</f>
+        <v>2982154.1590799987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="58">
+        <f>-35%*B7</f>
+        <v>-7620.1825000000645</v>
+      </c>
+      <c r="C8" s="58">
+        <f>-35%*C7</f>
+        <v>-1043753.9556779995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="62">
+        <f>B7+B8</f>
+        <v>14151.767500000122</v>
+      </c>
+      <c r="C9" s="62">
+        <f>C7+C8</f>
+        <v>1938400.2034019991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="64">
+        <f>B4+B9</f>
+        <v>154151.76750000013</v>
+      </c>
+      <c r="C10" s="64">
+        <f>C4+C9</f>
+        <v>1953251.9709019992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="66">
+        <v>2016</v>
+      </c>
+      <c r="D13" s="38">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="68">
+        <f>-B2</f>
+        <v>-500838</v>
+      </c>
+      <c r="C14" s="69">
+        <f>B10</f>
+        <v>154151.76750000013</v>
+      </c>
+      <c r="D14" s="69">
+        <f>C10</f>
+        <v>1953251.9709019992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="68">
+        <f>SUM(B14)</f>
+        <v>-500838</v>
+      </c>
+      <c r="C15" s="68">
+        <f>B15+C14</f>
+        <v>-346686.23249999987</v>
+      </c>
+      <c r="D15" s="71">
+        <f>C15+D14</f>
+        <v>1606565.7384019992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="76">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="70">
+        <v>0</v>
+      </c>
+      <c r="B20" s="68">
+        <f>B15</f>
+        <v>-500838</v>
+      </c>
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="70">
+        <v>1</v>
+      </c>
+      <c r="B21" s="68">
+        <f>C15</f>
+        <v>-346686.23249999987</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="70">
+        <v>2</v>
+      </c>
+      <c r="B22" s="71">
+        <f>D15</f>
+        <v>1606565.7384019992</v>
+      </c>
+      <c r="E22" s="26">
+        <f>D15</f>
+        <v>1606565.7384019992</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="72">
+        <f>IRR(B20:B22)</f>
+        <v>0.47804974264355615</v>
+      </c>
+      <c r="E23" s="26">
+        <f>-B21</f>
+        <v>346686.23249999987</v>
+      </c>
+      <c r="F23">
+        <f>E23*F22/E22</f>
+        <v>2.5895204226987025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="73">
+        <f>NPV(E19,B20:B22)</f>
+        <v>170224.1709510709</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,18 +2158,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="26">
-        <v>-358000</v>
+        <f>-'[2]Inversión Inicial PUM'!$E$31</f>
+        <v>-500838</v>
       </c>
       <c r="C3" s="26">
-        <f>Ganancias!B6</f>
-        <v>14151.767500000122</v>
+        <f>'Modelo Financiero'!C14</f>
+        <v>154151.76750000013</v>
       </c>
       <c r="D3" s="26">
-        <f>Ganancias!C6-Ganancias!C6*0.6</f>
-        <v>775360.08136079973</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
+        <f>Ganancias!C6</f>
+        <v>1938400.2034019991</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1702,7 +2175,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="19">
-        <v>0.23400000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1711,7 +2184,7 @@
       </c>
       <c r="B9" s="18">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>162650.296210161</v>
+        <v>814435.93368948763</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1720,7 +2193,7 @@
       </c>
       <c r="B10" s="19">
         <f>IRR(B3:D3)</f>
-        <v>0.49156697476814148</v>
+        <v>1.127215172418889</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1743,15 +2216,15 @@
       </c>
       <c r="B14">
         <f>B3</f>
-        <v>-358000</v>
+        <v>-500838</v>
       </c>
       <c r="C14">
         <f>B14+C3</f>
-        <v>-343848.23249999987</v>
-      </c>
-      <c r="D14">
+        <v>-346686.23249999987</v>
+      </c>
+      <c r="D14" s="26">
         <f>C14+D3</f>
-        <v>431511.84886079986</v>
+        <v>1591713.9709019992</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1762,7 +2235,7 @@
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>775360.08136079973</v>
+        <v>1938400.2034019991</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -1771,11 +2244,11 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
-        <v>343848.23249999987</v>
+        <v>346686.23249999987</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>5.3216291232820847</v>
+        <v>2.146220776647958</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1783,7 +2256,7 @@
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pasados ptos 6 y 7 al word general, pto 8 casi terminado
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
@@ -262,13 +262,13 @@
     <t>ROI</t>
   </si>
   <si>
-    <t>1 año y 3 meses</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ganancias Totales </t>
   </si>
   <si>
     <t>Fondo Final</t>
+  </si>
+  <si>
+    <t>1 año y 2 meses</t>
   </si>
 </sst>
 </file>
@@ -703,24 +703,6 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -751,6 +733,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,10 +815,10 @@
       <sheetData sheetId="2">
         <row r="4">
           <cell r="B4">
-            <v>4822844.05</v>
+            <v>4506241.5039999997</v>
           </cell>
           <cell r="C4">
-            <v>8767153.8409200013</v>
+            <v>9513409.3409200013</v>
           </cell>
         </row>
       </sheetData>
@@ -841,7 +841,7 @@
       <sheetName val="Costos fijos P1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="E3">
@@ -859,7 +859,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,12 +1143,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -1341,44 +1341,47 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1411,10 +1414,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="17">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="17">
         <v>1560</v>
@@ -1437,10 +1440,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="17">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="17">
         <v>3000</v>
@@ -1526,7 +1529,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D11" sqref="B10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,13 +1544,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
     </row>
     <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1578,11 +1581,11 @@
       </c>
       <c r="B3" s="16">
         <f>('Tipo Ingreso'!B3*'Volumenes Ingresos'!B4)*6</f>
-        <v>1056000</v>
+        <v>1248000</v>
       </c>
       <c r="C3" s="16">
         <f>('Tipo Ingreso'!B4*'Volumenes Ingresos'!C4)*6</f>
-        <v>472800</v>
+        <v>236400</v>
       </c>
       <c r="D3" s="16">
         <f>('Tipo Ingreso'!B5*'Volumenes Ingresos'!D4)</f>
@@ -1594,11 +1597,11 @@
       </c>
       <c r="F3" s="30">
         <f>SUM(B3:E3)</f>
-        <v>1910760</v>
+        <v>1866360</v>
       </c>
       <c r="H3" s="30">
         <f>F3/6</f>
-        <v>318460</v>
+        <v>311060</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1607,11 +1610,11 @@
       </c>
       <c r="B4" s="16">
         <f>('Tipo Ingreso'!C3*'Volumenes Ingresos'!B5)*6</f>
-        <v>1054080</v>
+        <v>1288320</v>
       </c>
       <c r="C4" s="16">
         <f>6*'Tipo Ingreso'!C4*'Volumenes Ingresos'!C5</f>
-        <v>865224</v>
+        <v>576816</v>
       </c>
       <c r="D4" s="16">
         <f>('Tipo Ingreso'!C5*'Volumenes Ingresos'!D5)*6</f>
@@ -1623,11 +1626,11 @@
       </c>
       <c r="F4" s="30">
         <f>SUM(B4:E4)</f>
-        <v>2933856</v>
+        <v>2879688</v>
       </c>
       <c r="H4" s="30">
         <f t="shared" ref="H4:H5" si="0">F4/6</f>
-        <v>488976</v>
+        <v>479948</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1706,7 +1709,7 @@
       </c>
       <c r="C11" s="31">
         <f>SUM(F3:F4)</f>
-        <v>4844616</v>
+        <v>4746048</v>
       </c>
       <c r="D11" s="32">
         <f>SUM(F5:F6)</f>
@@ -1753,7 +1756,7 @@
       </c>
       <c r="B2" s="8">
         <f>Ingresos!C11</f>
-        <v>4844616</v>
+        <v>4746048</v>
       </c>
       <c r="C2" s="8">
         <f>Ingresos!D11</f>
@@ -1766,11 +1769,11 @@
       </c>
       <c r="B3" s="29">
         <f>'[1]Gastos Resultado'!$B$4</f>
-        <v>4822844.05</v>
+        <v>4506241.5039999997</v>
       </c>
       <c r="C3" s="29">
         <f>'[1]Gastos Resultado'!$C$4</f>
-        <v>8767153.8409200013</v>
+        <v>9513409.3409200013</v>
       </c>
       <c r="G3" t="s">
         <v>48</v>
@@ -1785,11 +1788,11 @@
       </c>
       <c r="B4" s="36">
         <f>B2-B3</f>
-        <v>21771.950000000186</v>
+        <v>239806.49600000028</v>
       </c>
       <c r="C4" s="36">
         <f>C2-C3</f>
-        <v>2982154.1590799987</v>
+        <v>2235898.6590799987</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1798,11 +1801,11 @@
       </c>
       <c r="B5" s="40">
         <f>-(B4*H3)</f>
-        <v>-7620.1825000000645</v>
+        <v>-83932.273600000088</v>
       </c>
       <c r="C5" s="40">
         <f>-(C4*H3)</f>
-        <v>-1043753.9556779995</v>
+        <v>-782564.53067799949</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1811,11 +1814,11 @@
       </c>
       <c r="B6" s="41">
         <f>SUM(B4:B5)</f>
-        <v>14151.767500000122</v>
+        <v>155874.2224000002</v>
       </c>
       <c r="C6" s="42">
         <f>SUM(C4:C5)</f>
-        <v>1938400.2034019991</v>
+        <v>1453334.1284019994</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1828,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,131 +1846,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="44" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="57">
+      <c r="B2" s="51">
         <f>'[2]Inversión Inicial PUM'!$E$31</f>
         <v>500838</v>
       </c>
-      <c r="C2" s="57">
+      <c r="C2" s="51">
         <f>B10</f>
-        <v>154151.76750000013</v>
+        <v>295874.2224000002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="52">
         <f>-'[2]Inversión Inicial PUM'!$E$29</f>
         <v>-360838</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="52">
         <f>-('[2]Inversión Inicial PUM'!$E$3+'[2]Inversión Inicial PUM'!$E$3*40%)</f>
         <v>-139300</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="53">
         <f>B2+B3</f>
         <v>140000</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="53">
         <f>C2+C3</f>
-        <v>14851.767500000133</v>
+        <v>156574.2224000002</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="54">
         <f>Ganancias!B2</f>
-        <v>4844616</v>
-      </c>
-      <c r="C5" s="60">
+        <v>4746048</v>
+      </c>
+      <c r="C5" s="54">
         <f>Ganancias!C2</f>
         <v>11749308</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="52">
         <f>-Ganancias!B3</f>
-        <v>-4822844.05</v>
-      </c>
-      <c r="C6" s="58">
+        <v>-4506241.5039999997</v>
+      </c>
+      <c r="C6" s="52">
         <f>-Ganancias!C3</f>
-        <v>-8767153.8409200013</v>
+        <v>-9513409.3409200013</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="61">
+      <c r="B7" s="55">
         <f>B5+B6</f>
-        <v>21771.950000000186</v>
-      </c>
-      <c r="C7" s="61">
+        <v>239806.49600000028</v>
+      </c>
+      <c r="C7" s="55">
         <f>C5+C6</f>
-        <v>2982154.1590799987</v>
+        <v>2235898.6590799987</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="52">
         <f>-35%*B7</f>
-        <v>-7620.1825000000645</v>
-      </c>
-      <c r="C8" s="58">
+        <v>-83932.273600000088</v>
+      </c>
+      <c r="C8" s="52">
         <f>-35%*C7</f>
-        <v>-1043753.9556779995</v>
+        <v>-782564.53067799949</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="56">
+        <f>B7+B8</f>
+        <v>155874.2224000002</v>
+      </c>
+      <c r="C9" s="56">
+        <f>C7+C8</f>
+        <v>1453334.1284019994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="62">
-        <f>B7+B8</f>
-        <v>14151.767500000122</v>
-      </c>
-      <c r="C9" s="62">
-        <f>C7+C8</f>
-        <v>1938400.2034019991</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="64">
+      <c r="B10" s="58">
         <f>B4+B9</f>
-        <v>154151.76750000013</v>
-      </c>
-      <c r="C10" s="64">
+        <v>295874.2224000002</v>
+      </c>
+      <c r="C10" s="58">
         <f>C4+C9</f>
-        <v>1953251.9709019992</v>
+        <v>1609908.3508019997</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,10 +1983,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="66">
+      <c r="C13" s="60">
         <v>2016</v>
       </c>
       <c r="D13" s="38">
@@ -1991,37 +1994,37 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="68">
+      <c r="B14" s="62">
         <f>-B2</f>
         <v>-500838</v>
       </c>
-      <c r="C14" s="69">
+      <c r="C14" s="63">
         <f>B10</f>
-        <v>154151.76750000013</v>
-      </c>
-      <c r="D14" s="69">
+        <v>295874.2224000002</v>
+      </c>
+      <c r="D14" s="63">
         <f>C10</f>
-        <v>1953251.9709019992</v>
+        <v>1609908.3508019997</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="68">
+      <c r="B15" s="62">
         <f>SUM(B14)</f>
         <v>-500838</v>
       </c>
-      <c r="C15" s="68">
+      <c r="C15" s="62">
         <f>B15+C14</f>
-        <v>-346686.23249999987</v>
-      </c>
-      <c r="D15" s="71">
+        <v>-204963.7775999998</v>
+      </c>
+      <c r="D15" s="65">
         <f>C15+D14</f>
-        <v>1606565.7384019992</v>
+        <v>1404944.573202</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,47 +2043,47 @@
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="59" t="s">
         <v>57</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="76">
+      <c r="E19" s="70">
         <v>0.27400000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="70">
+      <c r="A20" s="64">
         <v>0</v>
       </c>
-      <c r="B20" s="68">
+      <c r="B20" s="62">
         <f>B15</f>
         <v>-500838</v>
       </c>
       <c r="C20" s="26"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="70">
+      <c r="A21" s="64">
         <v>1</v>
       </c>
-      <c r="B21" s="68">
+      <c r="B21" s="62">
         <f>C15</f>
-        <v>-346686.23249999987</v>
+        <v>-204963.7775999998</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="70">
+      <c r="A22" s="64">
         <v>2</v>
       </c>
-      <c r="B22" s="71">
+      <c r="B22" s="65">
         <f>D15</f>
-        <v>1606565.7384019992</v>
+        <v>1404944.573202</v>
       </c>
       <c r="E22" s="26">
         <f>D15</f>
-        <v>1606565.7384019992</v>
+        <v>1404944.573202</v>
       </c>
       <c r="F22">
         <v>12</v>
@@ -2090,34 +2093,34 @@
       <c r="A23" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="72">
+      <c r="B23" s="66">
         <f>IRR(B20:B22)</f>
-        <v>0.47804974264355615</v>
+        <v>0.48270170194957895</v>
       </c>
       <c r="E23" s="26">
         <f>-B21</f>
-        <v>346686.23249999987</v>
+        <v>204963.7775999998</v>
       </c>
       <c r="F23">
         <f>E23*F22/E22</f>
-        <v>2.5895204226987025</v>
+        <v>1.7506493694583398</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="73">
+      <c r="B24" s="67">
         <f>NPV(E19,B20:B22)</f>
-        <v>170224.1709510709</v>
+        <v>160036.15971279822</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="74" t="s">
-        <v>61</v>
+      <c r="B25" s="68" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2163,11 +2166,11 @@
       </c>
       <c r="C3" s="26">
         <f>'Modelo Financiero'!C14</f>
-        <v>154151.76750000013</v>
+        <v>295874.2224000002</v>
       </c>
       <c r="D3" s="26">
         <f>Ganancias!C6</f>
-        <v>1938400.2034019991</v>
+        <v>1453334.1284019994</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2184,7 +2187,7 @@
       </c>
       <c r="B9" s="18">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>814435.93368948763</v>
+        <v>626822.00343766971</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2193,7 +2196,7 @@
       </c>
       <c r="B10" s="19">
         <f>IRR(B3:D3)</f>
-        <v>1.127215172418889</v>
+        <v>1.0242671575489162</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2220,11 +2223,11 @@
       </c>
       <c r="C14">
         <f>B14+C3</f>
-        <v>-346686.23249999987</v>
+        <v>-204963.7775999998</v>
       </c>
       <c r="D14" s="26">
         <f>C14+D3</f>
-        <v>1591713.9709019992</v>
+        <v>1248370.3508019997</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2235,7 +2238,7 @@
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>1938400.2034019991</v>
+        <v>1453334.1284019994</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -2244,11 +2247,11 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
-        <v>346686.23249999987</v>
+        <v>204963.7775999998</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>2.146220776647958</v>
+        <v>1.692360540589789</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Punto 8 con qliksense, faltan escenarios
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Ganancias" sheetId="5" r:id="rId4"/>
     <sheet name="Modelo Financiero" sheetId="6" r:id="rId5"/>
     <sheet name="Indicadores Financieros" sheetId="4" r:id="rId6"/>
+    <sheet name="Escenario riesgo 1" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Mes</t>
   </si>
@@ -269,6 +270,12 @@
   </si>
   <si>
     <t>1 año y 2 meses</t>
+  </si>
+  <si>
+    <t>15% menos los gastos del primer año</t>
+  </si>
+  <si>
+    <t>1 año y 1 mes</t>
   </si>
 </sst>
 </file>
@@ -841,7 +848,7 @@
       <sheetName val="Costos fijos P1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="E3">
@@ -859,7 +866,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1384,7 +1391,7 @@
       <c r="H2" s="74"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>16</v>
@@ -1529,7 +1536,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="B10:D11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,4 +2273,307 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="51">
+        <f>'[2]Inversión Inicial PUM'!$E$31</f>
+        <v>500838</v>
+      </c>
+      <c r="C2" s="51">
+        <f>B10</f>
+        <v>442327.07128000009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="52">
+        <f>-'[2]Inversión Inicial PUM'!$E$29</f>
+        <v>-360838</v>
+      </c>
+      <c r="C3" s="52">
+        <f>-('[2]Inversión Inicial PUM'!$E$3+'[2]Inversión Inicial PUM'!$E$3*40%)</f>
+        <v>-139300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="53">
+        <f>B2+B3</f>
+        <v>140000</v>
+      </c>
+      <c r="C4" s="53">
+        <f>C2+C3</f>
+        <v>303027.07128000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="54">
+        <f>Ganancias!B2</f>
+        <v>4746048</v>
+      </c>
+      <c r="C5" s="54">
+        <f>Ganancias!C2</f>
+        <v>11749308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="52">
+        <f>-(Ganancias!B3-Ganancias!B3*0.05)</f>
+        <v>-4280929.4287999999</v>
+      </c>
+      <c r="C6" s="52">
+        <f>-Ganancias!C3</f>
+        <v>-9513409.3409200013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="55">
+        <f>B5+B6</f>
+        <v>465118.57120000012</v>
+      </c>
+      <c r="C7" s="55">
+        <f>C5+C6</f>
+        <v>2235898.6590799987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="52">
+        <f>-35%*B7</f>
+        <v>-162791.49992000003</v>
+      </c>
+      <c r="C8" s="52">
+        <f>-35%*C7</f>
+        <v>-782564.53067799949</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="56">
+        <f>B7+B8</f>
+        <v>302327.07128000009</v>
+      </c>
+      <c r="C9" s="56">
+        <f>C7+C8</f>
+        <v>1453334.1284019994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="58">
+        <f>B4+B9</f>
+        <v>442327.07128000009</v>
+      </c>
+      <c r="C10" s="58">
+        <f>C4+C9</f>
+        <v>1756361.1996819994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="60">
+        <v>2016</v>
+      </c>
+      <c r="D13" s="38">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="62">
+        <f>-B2</f>
+        <v>-500838</v>
+      </c>
+      <c r="C14" s="63">
+        <f>B10</f>
+        <v>442327.07128000009</v>
+      </c>
+      <c r="D14" s="63">
+        <f>C10</f>
+        <v>1756361.1996819994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="62">
+        <f>SUM(B14)</f>
+        <v>-500838</v>
+      </c>
+      <c r="C15" s="62">
+        <f>B15+C14</f>
+        <v>-58510.928719999909</v>
+      </c>
+      <c r="D15" s="65">
+        <f>C15+D14</f>
+        <v>1697850.2709619994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="70">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="64">
+        <v>0</v>
+      </c>
+      <c r="B20" s="62">
+        <f>B15</f>
+        <v>-500838</v>
+      </c>
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="64">
+        <v>1</v>
+      </c>
+      <c r="B21" s="62">
+        <f>C15</f>
+        <v>-58510.928719999909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="64">
+        <v>2</v>
+      </c>
+      <c r="B22" s="65">
+        <f>D15</f>
+        <v>1697850.2709619994</v>
+      </c>
+      <c r="E22" s="26">
+        <f>D15</f>
+        <v>1697850.2709619994</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="66">
+        <f>IRR(B20:B22)</f>
+        <v>0.78371371856494365</v>
+      </c>
+      <c r="E23" s="26">
+        <f>-B21</f>
+        <v>58510.928719999909</v>
+      </c>
+      <c r="F23">
+        <f>E23*F22/E22</f>
+        <v>0.41354126252968848</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="67">
+        <f>NPV(E19,B20:B22)</f>
+        <v>391918.78855847515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregado pto 8 y 9 a word general
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Borrador Ingresos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Ingreso" sheetId="2" r:id="rId1"/>
@@ -19,10 +19,12 @@
     <sheet name="Modelo Financiero" sheetId="6" r:id="rId5"/>
     <sheet name="Indicadores Financieros" sheetId="4" r:id="rId6"/>
     <sheet name="Escenario riesgo 1" sheetId="7" r:id="rId7"/>
+    <sheet name="Escenario de riesgo 2" sheetId="8" r:id="rId8"/>
+    <sheet name="Escenario riesgo 3" sheetId="9" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
   <si>
     <t>Mes</t>
   </si>
@@ -276,6 +278,18 @@
   </si>
   <si>
     <t>1 año y 1 mes</t>
+  </si>
+  <si>
+    <t>15% menos de ingresos en el segundo año</t>
+  </si>
+  <si>
+    <t>1 año y 10 meses</t>
+  </si>
+  <si>
+    <t>10% aumento de egresos en el primer año</t>
+  </si>
+  <si>
+    <t>1 año y 8 meses</t>
   </si>
 </sst>
 </file>
@@ -2279,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2576,4 +2590,611 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="51">
+        <f>'[2]Inversión Inicial PUM'!$E$31</f>
+        <v>500838</v>
+      </c>
+      <c r="C2" s="51">
+        <f>B10</f>
+        <v>295874.2224000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="52">
+        <f>-'[2]Inversión Inicial PUM'!$E$29</f>
+        <v>-360838</v>
+      </c>
+      <c r="C3" s="52">
+        <f>-('[2]Inversión Inicial PUM'!$E$3+'[2]Inversión Inicial PUM'!$E$3*40%)</f>
+        <v>-139300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="53">
+        <f>B2+B3</f>
+        <v>140000</v>
+      </c>
+      <c r="C4" s="53">
+        <f>C2+C3</f>
+        <v>156574.2224000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="54">
+        <f>Ganancias!B2</f>
+        <v>4746048</v>
+      </c>
+      <c r="C5" s="54">
+        <f>Ganancias!C2-(Ganancias!C2*0.15)</f>
+        <v>9986911.8000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="52">
+        <f>-(Ganancias!B3)</f>
+        <v>-4506241.5039999997</v>
+      </c>
+      <c r="C6" s="52">
+        <f>-Ganancias!C3</f>
+        <v>-9513409.3409200013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="55">
+        <f>B5+B6</f>
+        <v>239806.49600000028</v>
+      </c>
+      <c r="C7" s="55">
+        <f>C5+C6</f>
+        <v>473502.45907999948</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="52">
+        <f>-35%*B7</f>
+        <v>-83932.273600000088</v>
+      </c>
+      <c r="C8" s="52">
+        <f>-35%*C7</f>
+        <v>-165725.86067799979</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="56">
+        <f>B7+B8</f>
+        <v>155874.2224000002</v>
+      </c>
+      <c r="C9" s="56">
+        <f>C7+C8</f>
+        <v>307776.59840199968</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="58">
+        <f>B4+B9</f>
+        <v>295874.2224000002</v>
+      </c>
+      <c r="C10" s="58">
+        <f>C4+C9</f>
+        <v>464350.82080199989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="60">
+        <v>2016</v>
+      </c>
+      <c r="D13" s="38">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="62">
+        <f>-B2</f>
+        <v>-500838</v>
+      </c>
+      <c r="C14" s="63">
+        <f>B10</f>
+        <v>295874.2224000002</v>
+      </c>
+      <c r="D14" s="63">
+        <f>C10</f>
+        <v>464350.82080199989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="62">
+        <f>SUM(B14)</f>
+        <v>-500838</v>
+      </c>
+      <c r="C15" s="62">
+        <f>B15+C14</f>
+        <v>-204963.7775999998</v>
+      </c>
+      <c r="D15" s="65">
+        <f>C15+D14</f>
+        <v>259387.04320200009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="70">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="64">
+        <v>0</v>
+      </c>
+      <c r="B20" s="62">
+        <f>B15</f>
+        <v>-500838</v>
+      </c>
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="64">
+        <v>1</v>
+      </c>
+      <c r="B21" s="62">
+        <f>C15</f>
+        <v>-204963.7775999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="64">
+        <v>2</v>
+      </c>
+      <c r="B22" s="65">
+        <f>D15</f>
+        <v>259387.04320200009</v>
+      </c>
+      <c r="E22" s="26">
+        <f>D15</f>
+        <v>259387.04320200009</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="66">
+        <f>IRR(B20:B22)</f>
+        <v>-0.45643919661249133</v>
+      </c>
+      <c r="E23" s="26">
+        <f>-B21</f>
+        <v>204963.7775999998</v>
+      </c>
+      <c r="F23">
+        <f>E23*F22/E22</f>
+        <v>9.4822212429654318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="67">
+        <f>NPV(E19,B20:B22)</f>
+        <v>-393962.38052430557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="51">
+        <f>'[2]Inversión Inicial PUM'!$E$31</f>
+        <v>500838</v>
+      </c>
+      <c r="C2" s="51">
+        <f>B10</f>
+        <v>2968.5246400003671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="52">
+        <f>-'[2]Inversión Inicial PUM'!$E$29</f>
+        <v>-360838</v>
+      </c>
+      <c r="C3" s="52">
+        <f>-('[2]Inversión Inicial PUM'!$E$3+'[2]Inversión Inicial PUM'!$E$3*40%)</f>
+        <v>-139300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="53">
+        <f>B2+B3</f>
+        <v>140000</v>
+      </c>
+      <c r="C4" s="53">
+        <f>C2+C3</f>
+        <v>-136331.47535999963</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="54">
+        <f>Ganancias!B2</f>
+        <v>4746048</v>
+      </c>
+      <c r="C5" s="54">
+        <f>Ganancias!C2</f>
+        <v>11749308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="52">
+        <f>-(Ganancias!B3+Ganancias!B3*0.1)</f>
+        <v>-4956865.6543999994</v>
+      </c>
+      <c r="C6" s="52">
+        <f>-Ganancias!C3</f>
+        <v>-9513409.3409200013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="55">
+        <f>B5+B6</f>
+        <v>-210817.65439999942</v>
+      </c>
+      <c r="C7" s="55">
+        <f>C5+C6</f>
+        <v>2235898.6590799987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="52">
+        <f>-35%*B7</f>
+        <v>73786.179039999784</v>
+      </c>
+      <c r="C8" s="52">
+        <f>-35%*C7</f>
+        <v>-782564.53067799949</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="56">
+        <f>B7+B8</f>
+        <v>-137031.47535999963</v>
+      </c>
+      <c r="C9" s="56">
+        <f>C7+C8</f>
+        <v>1453334.1284019994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="58">
+        <f>B4+B9</f>
+        <v>2968.5246400003671</v>
+      </c>
+      <c r="C10" s="58">
+        <f>C4+C9</f>
+        <v>1317002.6530419998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="60">
+        <v>2016</v>
+      </c>
+      <c r="D13" s="38">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="62">
+        <f>-B2</f>
+        <v>-500838</v>
+      </c>
+      <c r="C14" s="63">
+        <f>B10</f>
+        <v>2968.5246400003671</v>
+      </c>
+      <c r="D14" s="63">
+        <f>C10</f>
+        <v>1317002.6530419998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="62">
+        <f>SUM(B14)</f>
+        <v>-500838</v>
+      </c>
+      <c r="C15" s="62">
+        <f>B15+C14</f>
+        <v>-497869.47535999963</v>
+      </c>
+      <c r="D15" s="65">
+        <f>C15+D14</f>
+        <v>819133.17768200021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="70">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="64">
+        <v>0</v>
+      </c>
+      <c r="B20" s="62">
+        <f>B15</f>
+        <v>-500838</v>
+      </c>
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="64">
+        <v>1</v>
+      </c>
+      <c r="B21" s="62">
+        <f>C15</f>
+        <v>-497869.47535999963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="64">
+        <v>2</v>
+      </c>
+      <c r="B22" s="65">
+        <f>D15</f>
+        <v>819133.17768200021</v>
+      </c>
+      <c r="E22" s="26">
+        <f>D15</f>
+        <v>819133.17768200021</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="66">
+        <f>IRR(B20:B22)</f>
+        <v>-0.12496849933655285</v>
+      </c>
+      <c r="E23" s="26">
+        <f>-B21</f>
+        <v>497869.47535999963</v>
+      </c>
+      <c r="F23">
+        <f>E23*F22/E22</f>
+        <v>7.2936048338642196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="67">
+        <f>NPV(E19,B20:B22)</f>
+        <v>-303729.09797855624</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>